<commit_message>
End of semester additions for Renal Project
</commit_message>
<xml_diff>
--- a/Data Science/202003015_PD_trends_V1.xlsx
+++ b/Data Science/202003015_PD_trends_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Data\ME_Renal\Data Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54163882-56A5-4FDD-AA52-C3C2CFDFAF94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A02016-0450-4B33-9325-AE03D70C1525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27825" windowHeight="16440" xr2:uid="{209DCC94-64CE-4145-AD13-CB94F44A4FA8}"/>
+    <workbookView xWindow="2865" yWindow="2430" windowWidth="22605" windowHeight="13515" xr2:uid="{209DCC94-64CE-4145-AD13-CB94F44A4FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6415,6 +6415,971 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
+              <a:t>ESRD Modality 2000-2016</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12216868927415382"/>
+          <c:y val="0.12603588503050772"/>
+          <c:w val="0.85532653018939664"/>
+          <c:h val="0.76503518881762933"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Hemodialysis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$6:$A$22</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$6:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$M$6:$M$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$M$6:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>254080</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>267456</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>279656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>291105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>302457</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>313384</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>326344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>338845</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>352500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>367250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>380354</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>390383</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>402755</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>416088</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>430997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>445354</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>457957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8DFD-4021-9D3B-A9265518110C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Peritoneal DIalysis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$6:$A$22</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$6:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$O$6:$O$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$O$6:$O$22</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>27281</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27748</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28065</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28317</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28338</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28708</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28955</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30119</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36083</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39784</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43880</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>46772</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49492</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8DFD-4021-9D3B-A9265518110C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Transplant</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$6:$A$22</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$6:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$Q$6:$Q$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$Q$6:$Q$22</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>107848</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>121314</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128133</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>135519</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142910</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150595</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>157860</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>164848</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>171648</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>178285</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>184643</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>190454</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196289</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>201914</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>208032</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>215061</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8DFD-4021-9D3B-A9265518110C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="677580048"/>
+        <c:axId val="677581008"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="677580048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                  <a:t>YEAR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="677581008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="677581008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="24000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                  <a:t>Patient Population</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="677580048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6536,6 +7501,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8559,6 +9564,502 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="283">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -8704,6 +10205,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>108858</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>193134</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>115201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1C8767-66D5-44E2-815E-EB81FFEDABF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9792,9 +11331,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB5B574-9F3F-417A-BD46-D7C409446916}">
   <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="62" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="35" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BK17" sqref="BK17"/>
+      <selection pane="topRight" activeCell="AQ76" sqref="AQ76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>